<commit_message>
week3 - seesion 1
</commit_message>
<xml_diff>
--- a/speed_up.xlsx
+++ b/speed_up.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="C++" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t xml:space="preserve">Serial</t>
   </si>
@@ -155,35 +156,40 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -191,18 +197,18 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -215,4 +221,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1592.43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>617.827</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1443.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
week5 - session 1
</commit_message>
<xml_diff>
--- a/speed_up.xlsx
+++ b/speed_up.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t xml:space="preserve">Serial C</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">SpeedUp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fork-Join</t>
   </si>
   <si>
     <t xml:space="preserve">PI</t>
@@ -69,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -91,6 +94,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,7 +161,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,21 +190,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,10 +225,16 @@
       <c r="G1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2323.5695</v>
@@ -217,18 +243,24 @@
         <v>1592.43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3091.5525</v>
@@ -239,17 +271,24 @@
       <c r="D3" s="2" t="n">
         <v>162.6</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="5" t="n">
         <v>86.9</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <f aca="false">D3/F3</f>
         <v>1.87111622554661</v>
       </c>
+      <c r="H3" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">D3/H3</f>
+        <v>1.91294117647059</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>373.6993</v>
@@ -260,17 +299,24 @@
       <c r="D4" s="2" t="n">
         <v>139</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>126.4</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <f aca="false">D4/F4</f>
         <v>1.0996835443038</v>
       </c>
+      <c r="H4" s="5" t="n">
+        <v>122</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">D4/H4</f>
+        <v>1.13934426229508</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>565.8621</v>
@@ -281,17 +327,25 @@
       <c r="D5" s="2" t="n">
         <v>412.6</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>199.3</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <f aca="false">D5/F5</f>
         <v>2.07024586051179</v>
       </c>
+      <c r="H5" s="5" t="n">
+        <v>102.2</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <f aca="false">D5/H5</f>
+        <v>4.03718199608611</v>
+      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>208.9001</v>
@@ -302,55 +356,61 @@
       <c r="D6" s="2" t="n">
         <v>200.6</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="5" t="n">
         <v>115</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="5" t="n">
         <f aca="false">D6/F6</f>
         <v>1.74434782608696</v>
       </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>978.1137</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="5" t="n">
         <v>1054.61</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>276.8</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>111</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="5" t="n">
         <f aca="false">D7/F7</f>
         <v>2.49369369369369</v>
       </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4333.9</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>636.3</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <f aca="false">D8/F8</f>
         <v>6.81109539525381</v>
       </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
week 6 - session 1
</commit_message>
<xml_diff>
--- a/speed_up.xlsx
+++ b/speed_up.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Serial C</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fork-Join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpeedUṕ</t>
   </si>
   <si>
     <t xml:space="preserve">PI</t>
@@ -208,20 +214,20 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,10 +252,16 @@
       <c r="I1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2323.5695</v>
@@ -274,10 +286,17 @@
         <f aca="false">D2/H2</f>
         <v>4.41807228915663</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <v>768.09</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <f aca="false">B2/J2</f>
+        <v>3.02512661276673</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>3091.5525</v>
@@ -291,7 +310,7 @@
       <c r="F3" s="5" t="n">
         <v>86.9</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="2" t="n">
         <f aca="false">D3/F3</f>
         <v>1.87111622554661</v>
       </c>
@@ -302,10 +321,17 @@
         <f aca="false">D3/H3</f>
         <v>1.84562996594779</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>1423.99</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <f aca="false">B3/J3</f>
+        <v>2.17104930512152</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>373.6993</v>
@@ -333,7 +359,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>565.8621</v>
@@ -362,7 +388,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>208.9001</v>
@@ -390,7 +416,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>978.1137</v>
@@ -418,13 +444,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4333.9</v>

</xml_diff>

<commit_message>
week 6 - session 1a
</commit_message>
<xml_diff>
--- a/speed_up.xlsx
+++ b/speed_up.xlsx
@@ -214,7 +214,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -352,9 +352,16 @@
       <c r="H4" s="5" t="n">
         <v>122</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="2" t="n">
         <f aca="false">D4/H4</f>
         <v>1.13934426229508</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>217.43</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <f aca="false">B4/J4</f>
+        <v>1.71871084946879</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>